<commit_message>
Preparation of regional data for germany
- creating for loop to loop over keys in dictionary and organize data of dataframes in one go
- preparing code to include all the regional data for germany
</commit_message>
<xml_diff>
--- a/Bevölkerungsentwicklung_Deutschland_Bundesländer.xlsx
+++ b/Bevölkerungsentwicklung_Deutschland_Bundesländer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabie\Universität St.Gallen\Software-Engineering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F37E534F-AD9B-4426-A7F8-5106A4BDC15D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA122FA6-DD24-4D1C-B837-94C5D8724194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -138,7 +138,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -193,19 +193,6 @@
       <top style="thin">
         <color indexed="8"/>
       </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
       <bottom style="medium">
         <color indexed="8"/>
       </bottom>
@@ -215,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -223,17 +210,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -248,6 +226,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -564,8 +545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96950B6F-A372-45FC-9001-9A770A3B88BF}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -584,67 +565,67 @@
     <col min="18" max="18" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="N1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="R1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="S1" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5">
+      <c r="A2" s="9">
         <v>2020</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -653,171 +634,175 @@
       <c r="C2" s="1">
         <v>83155031</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="4">
         <v>2910875</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="4">
         <v>1852478</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="4">
         <v>8003421</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="4">
         <v>680130</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="4">
         <v>17925570</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="4">
         <v>6293154</v>
       </c>
-      <c r="J2" s="7">
+      <c r="J2" s="4">
         <v>4098391</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="4">
         <v>11103043</v>
       </c>
-      <c r="L2" s="7">
+      <c r="L2" s="4">
         <v>13140183</v>
       </c>
-      <c r="M2" s="7">
+      <c r="M2" s="4">
         <v>983991</v>
       </c>
-      <c r="N2" s="7">
+      <c r="N2" s="4">
         <v>3664088</v>
       </c>
-      <c r="O2" s="7">
+      <c r="O2" s="4">
         <v>2531071</v>
       </c>
-      <c r="P2" s="7">
+      <c r="P2" s="4">
         <v>1610774</v>
       </c>
-      <c r="Q2" s="7">
+      <c r="Q2" s="4">
         <v>4056941</v>
       </c>
-      <c r="R2" s="7">
+      <c r="R2" s="4">
         <v>2180684</v>
       </c>
-      <c r="S2" s="7">
+      <c r="S2" s="4">
         <v>2120237</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4"/>
+      <c r="A3" s="9">
+        <v>2020</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1">
         <v>41026519</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="4">
         <v>1425649</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="4">
         <v>906933</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="4">
         <v>3951456</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="4">
         <v>336390</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="4">
         <v>8794888</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="4">
         <v>3108408</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="4">
         <v>2026105</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="4">
         <v>5516636</v>
       </c>
-      <c r="L3" s="7">
+      <c r="L3" s="4">
         <v>6512595</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="4">
         <v>483001</v>
       </c>
-      <c r="N3" s="7">
+      <c r="N3" s="4">
         <v>1802038</v>
       </c>
-      <c r="O3" s="7">
+      <c r="O3" s="4">
         <v>1248050</v>
       </c>
-      <c r="P3" s="7">
+      <c r="P3" s="4">
         <v>793537</v>
       </c>
-      <c r="Q3" s="7">
+      <c r="Q3" s="4">
         <v>1999026</v>
       </c>
-      <c r="R3" s="7">
+      <c r="R3" s="4">
         <v>1072595</v>
       </c>
-      <c r="S3" s="7">
+      <c r="S3" s="4">
         <v>1049212</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="4"/>
+      <c r="A4" s="9">
+        <v>2020</v>
+      </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1">
         <v>42128512</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="4">
         <v>1485226</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="4">
         <v>945545</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="4">
         <v>4051965</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="4">
         <v>343740</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="4">
         <v>9130682</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="4">
         <v>3184746</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="4">
         <v>2072286</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="4">
         <v>5586407</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="4">
         <v>6627588</v>
       </c>
-      <c r="M4" s="7">
+      <c r="M4" s="4">
         <v>500990</v>
       </c>
-      <c r="N4" s="7">
+      <c r="N4" s="4">
         <v>1862050</v>
       </c>
-      <c r="O4" s="7">
+      <c r="O4" s="4">
         <v>1283021</v>
       </c>
-      <c r="P4" s="7">
+      <c r="P4" s="4">
         <v>817237</v>
       </c>
-      <c r="Q4" s="7">
+      <c r="Q4" s="4">
         <v>2057915</v>
       </c>
-      <c r="R4" s="7">
+      <c r="R4" s="4">
         <v>1108089</v>
       </c>
-      <c r="S4" s="7">
+      <c r="S4" s="4">
         <v>1071025</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5">
+      <c r="A5" s="9">
         <v>2019</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -826,171 +811,175 @@
       <c r="C5" s="1">
         <v>83166711</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="4">
         <v>2903773</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="4">
         <v>1847253</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="4">
         <v>7993608</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="4">
         <v>681202</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="4">
         <v>17947221</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="4">
         <v>6288080</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="4">
         <v>4093903</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="4">
         <v>11100394</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="4">
         <v>13124737</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="4">
         <v>986887</v>
       </c>
-      <c r="N5" s="7">
+      <c r="N5" s="4">
         <v>3669491</v>
       </c>
-      <c r="O5" s="7">
+      <c r="O5" s="4">
         <v>2521893</v>
       </c>
-      <c r="P5" s="7">
+      <c r="P5" s="4">
         <v>1608138</v>
       </c>
-      <c r="Q5" s="7">
+      <c r="Q5" s="4">
         <v>4071971</v>
       </c>
-      <c r="R5" s="7">
+      <c r="R5" s="4">
         <v>2194782</v>
       </c>
-      <c r="S5" s="7">
+      <c r="S5" s="4">
         <v>2133378</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4"/>
+      <c r="A6" s="9">
+        <v>2019</v>
+      </c>
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="1">
         <v>41037613</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="4">
         <v>1422883</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="4">
         <v>903974</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="4">
         <v>3947571</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="4">
         <v>337001</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="4">
         <v>8805974</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="4">
         <v>3105260</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="4">
         <v>2023004</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="4">
         <v>5516440</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="4">
         <v>6507691</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6" s="4">
         <v>484419</v>
       </c>
-      <c r="N6" s="7">
+      <c r="N6" s="4">
         <v>1804273</v>
       </c>
-      <c r="O6" s="7">
+      <c r="O6" s="4">
         <v>1243931</v>
       </c>
-      <c r="P6" s="7">
+      <c r="P6" s="4">
         <v>792612</v>
       </c>
-      <c r="Q6" s="7">
+      <c r="Q6" s="4">
         <v>2006722</v>
       </c>
-      <c r="R6" s="7">
+      <c r="R6" s="4">
         <v>1079862</v>
       </c>
-      <c r="S6" s="7">
+      <c r="S6" s="4">
         <v>1055996</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4"/>
+      <c r="A7" s="9">
+        <v>2019</v>
+      </c>
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="1">
         <v>42129098</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="4">
         <v>1480890</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="4">
         <v>943279</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="4">
         <v>4046037</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="4">
         <v>344201</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="4">
         <v>9141247</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="4">
         <v>3182820</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="4">
         <v>2070899</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="4">
         <v>5583954</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L7" s="4">
         <v>6617046</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="4">
         <v>502468</v>
       </c>
-      <c r="N7" s="7">
+      <c r="N7" s="4">
         <v>1865218</v>
       </c>
-      <c r="O7" s="7">
+      <c r="O7" s="4">
         <v>1277962</v>
       </c>
-      <c r="P7" s="7">
+      <c r="P7" s="4">
         <v>815526</v>
       </c>
-      <c r="Q7" s="7">
+      <c r="Q7" s="4">
         <v>2065249</v>
       </c>
-      <c r="R7" s="7">
+      <c r="R7" s="4">
         <v>1114920</v>
       </c>
-      <c r="S7" s="7">
+      <c r="S7" s="4">
         <v>1077382</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="5">
+      <c r="A8" s="9">
         <v>2018</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -999,171 +988,175 @@
       <c r="C8" s="1">
         <v>83019213</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="4">
         <v>2896712</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="4">
         <v>1841179</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="4">
         <v>7982448</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="4">
         <v>682986</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="4">
         <v>17932651</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="4">
         <v>6265809</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="4">
         <v>4084844</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="4">
         <v>11069533</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L8" s="4">
         <v>13076721</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="4">
         <v>990509</v>
       </c>
-      <c r="N8" s="7">
+      <c r="N8" s="4">
         <v>3644826</v>
       </c>
-      <c r="O8" s="7">
+      <c r="O8" s="4">
         <v>2511917</v>
       </c>
-      <c r="P8" s="7">
+      <c r="P8" s="4">
         <v>1609675</v>
       </c>
-      <c r="Q8" s="7">
+      <c r="Q8" s="4">
         <v>4077937</v>
       </c>
-      <c r="R8" s="7">
+      <c r="R8" s="4">
         <v>2208321</v>
       </c>
-      <c r="S8" s="7">
+      <c r="S8" s="4">
         <v>2143145</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4"/>
+      <c r="A9" s="9">
+        <v>2018</v>
+      </c>
       <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="1">
         <v>40966691</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="4">
         <v>1419457</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="4">
         <v>902048</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="4">
         <v>3943243</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="4">
         <v>338035</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="4">
         <v>8798631</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="4">
         <v>3093044</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="4">
         <v>2017576</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K9" s="4">
         <v>5501693</v>
       </c>
-      <c r="L9" s="7">
+      <c r="L9" s="4">
         <v>6483793</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="4">
         <v>486159</v>
       </c>
-      <c r="N9" s="7">
+      <c r="N9" s="4">
         <v>1792801</v>
       </c>
-      <c r="O9" s="7">
+      <c r="O9" s="4">
         <v>1239460</v>
       </c>
-      <c r="P9" s="7">
+      <c r="P9" s="4">
         <v>793639</v>
       </c>
-      <c r="Q9" s="7">
+      <c r="Q9" s="4">
         <v>2009619</v>
       </c>
-      <c r="R9" s="7">
+      <c r="R9" s="4">
         <v>1086679</v>
       </c>
-      <c r="S9" s="7">
+      <c r="S9" s="4">
         <v>1060814</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4"/>
+      <c r="A10" s="9">
+        <v>2018</v>
+      </c>
       <c r="B10" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="1">
         <v>42052522</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="4">
         <v>1477255</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="4">
         <v>939131</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="4">
         <v>4039205</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="4">
         <v>344951</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="4">
         <v>9134020</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="4">
         <v>3172765</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="4">
         <v>2067268</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K10" s="4">
         <v>5567840</v>
       </c>
-      <c r="L10" s="7">
+      <c r="L10" s="4">
         <v>6592928</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10" s="4">
         <v>504350</v>
       </c>
-      <c r="N10" s="7">
+      <c r="N10" s="4">
         <v>1852025</v>
       </c>
-      <c r="O10" s="7">
+      <c r="O10" s="4">
         <v>1272457</v>
       </c>
-      <c r="P10" s="7">
+      <c r="P10" s="4">
         <v>816036</v>
       </c>
-      <c r="Q10" s="7">
+      <c r="Q10" s="4">
         <v>2068318</v>
       </c>
-      <c r="R10" s="7">
+      <c r="R10" s="4">
         <v>1121642</v>
       </c>
-      <c r="S10" s="7">
+      <c r="S10" s="4">
         <v>1082331</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="5">
+      <c r="A11" s="9">
         <v>2017</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1172,171 +1165,175 @@
       <c r="C11" s="1">
         <v>82792351</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="4">
         <v>2889821</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="4">
         <v>1830584</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="4">
         <v>7962775</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="4">
         <v>681032</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="4">
         <v>17912134</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="4">
         <v>6243262</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="4">
         <v>4073679</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="4">
         <v>11023425</v>
       </c>
-      <c r="L11" s="7">
+      <c r="L11" s="4">
         <v>12997204</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11" s="4">
         <v>994187</v>
       </c>
-      <c r="N11" s="7">
+      <c r="N11" s="4">
         <v>3613495</v>
       </c>
-      <c r="O11" s="7">
+      <c r="O11" s="4">
         <v>2504040</v>
       </c>
-      <c r="P11" s="7">
+      <c r="P11" s="4">
         <v>1611119</v>
       </c>
-      <c r="Q11" s="7">
+      <c r="Q11" s="4">
         <v>4081308</v>
       </c>
-      <c r="R11" s="7">
+      <c r="R11" s="4">
         <v>2223081</v>
       </c>
-      <c r="S11" s="7">
+      <c r="S11" s="4">
         <v>2151205</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4"/>
+      <c r="A12" s="9">
+        <v>2017</v>
+      </c>
       <c r="B12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="1">
         <v>40843565</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="4">
         <v>1416535</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="4">
         <v>897207</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="4">
         <v>3931876</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G12" s="4">
         <v>336665</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="4">
         <v>8787579</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="4">
         <v>3081636</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="4">
         <v>2011123</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="4">
         <v>5477341</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="4">
         <v>6438503</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="4">
         <v>487895</v>
       </c>
-      <c r="N12" s="7">
+      <c r="N12" s="4">
         <v>1776267</v>
       </c>
-      <c r="O12" s="7">
+      <c r="O12" s="4">
         <v>1235971</v>
       </c>
-      <c r="P12" s="7">
+      <c r="P12" s="4">
         <v>794873</v>
       </c>
-      <c r="Q12" s="7">
+      <c r="Q12" s="4">
         <v>2010214</v>
       </c>
-      <c r="R12" s="7">
+      <c r="R12" s="4">
         <v>1094876</v>
       </c>
-      <c r="S12" s="7">
+      <c r="S12" s="4">
         <v>1065004</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="4"/>
+      <c r="A13" s="9">
+        <v>2017</v>
+      </c>
       <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="1">
         <v>41948786</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="4">
         <v>1473286</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="4">
         <v>933377</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="4">
         <v>4030899</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="4">
         <v>344367</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="4">
         <v>9124555</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="4">
         <v>3161626</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="4">
         <v>2062556</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K13" s="4">
         <v>5546084</v>
       </c>
-      <c r="L13" s="7">
+      <c r="L13" s="4">
         <v>6558701</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M13" s="4">
         <v>506292</v>
       </c>
-      <c r="N13" s="7">
+      <c r="N13" s="4">
         <v>1837228</v>
       </c>
-      <c r="O13" s="7">
+      <c r="O13" s="4">
         <v>1268069</v>
       </c>
-      <c r="P13" s="7">
+      <c r="P13" s="4">
         <v>816246</v>
       </c>
-      <c r="Q13" s="7">
+      <c r="Q13" s="4">
         <v>2071094</v>
       </c>
-      <c r="R13" s="7">
+      <c r="R13" s="4">
         <v>1128205</v>
       </c>
-      <c r="S13" s="7">
+      <c r="S13" s="4">
         <v>1086201</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="5">
+      <c r="A14" s="9">
         <v>2016</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1345,171 +1342,175 @@
       <c r="C14" s="1">
         <v>82521653</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="4">
         <v>2881926</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="4">
         <v>1810438</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="4">
         <v>7945685</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="4">
         <v>678753</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="4">
         <v>17890100</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I14" s="4">
         <v>6213088</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J14" s="4">
         <v>4066053</v>
       </c>
-      <c r="K14" s="7">
+      <c r="K14" s="4">
         <v>10951893</v>
       </c>
-      <c r="L14" s="7">
+      <c r="L14" s="4">
         <v>12930751</v>
       </c>
-      <c r="M14" s="7">
+      <c r="M14" s="4">
         <v>996651</v>
       </c>
-      <c r="N14" s="7">
+      <c r="N14" s="4">
         <v>3574830</v>
       </c>
-      <c r="O14" s="7">
+      <c r="O14" s="4">
         <v>2494648</v>
       </c>
-      <c r="P14" s="7">
+      <c r="P14" s="4">
         <v>1610674</v>
       </c>
-      <c r="Q14" s="7">
+      <c r="Q14" s="4">
         <v>4081783</v>
       </c>
-      <c r="R14" s="7">
+      <c r="R14" s="4">
         <v>2236252</v>
       </c>
-      <c r="S14" s="7">
+      <c r="S14" s="4">
         <v>2158128</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="4"/>
+      <c r="A15" s="9">
+        <v>2016</v>
+      </c>
       <c r="B15" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="1">
         <v>40697118</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="4">
         <v>1412665</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="4">
         <v>886289</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="4">
         <v>3923396</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="4">
         <v>335474</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="4">
         <v>8776760</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="4">
         <v>3066957</v>
       </c>
-      <c r="J15" s="7">
+      <c r="J15" s="4">
         <v>2006503</v>
       </c>
-      <c r="K15" s="7">
+      <c r="K15" s="4">
         <v>5435665</v>
       </c>
-      <c r="L15" s="7">
+      <c r="L15" s="4">
         <v>6400820</v>
       </c>
-      <c r="M15" s="7">
+      <c r="M15" s="4">
         <v>489416</v>
       </c>
-      <c r="N15" s="7">
+      <c r="N15" s="4">
         <v>1755700</v>
       </c>
-      <c r="O15" s="7">
+      <c r="O15" s="4">
         <v>1231683</v>
       </c>
-      <c r="P15" s="7">
+      <c r="P15" s="4">
         <v>795467</v>
       </c>
-      <c r="Q15" s="7">
+      <c r="Q15" s="4">
         <v>2009991</v>
       </c>
-      <c r="R15" s="7">
+      <c r="R15" s="4">
         <v>1102454</v>
       </c>
-      <c r="S15" s="7">
+      <c r="S15" s="4">
         <v>1067878</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="4"/>
+      <c r="A16" s="9">
+        <v>2016</v>
+      </c>
       <c r="B16" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="1">
         <v>41824535</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16" s="4">
         <v>1469261</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="4">
         <v>924149</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="4">
         <v>4022289</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="4">
         <v>343279</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="4">
         <v>9113340</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16" s="4">
         <v>3146131</v>
       </c>
-      <c r="J16" s="7">
+      <c r="J16" s="4">
         <v>2059550</v>
       </c>
-      <c r="K16" s="7">
+      <c r="K16" s="4">
         <v>5516228</v>
       </c>
-      <c r="L16" s="7">
+      <c r="L16" s="4">
         <v>6529931</v>
       </c>
-      <c r="M16" s="7">
+      <c r="M16" s="4">
         <v>507235</v>
       </c>
-      <c r="N16" s="7">
+      <c r="N16" s="4">
         <v>1819130</v>
       </c>
-      <c r="O16" s="7">
+      <c r="O16" s="4">
         <v>1262965</v>
       </c>
-      <c r="P16" s="7">
+      <c r="P16" s="4">
         <v>815207</v>
       </c>
-      <c r="Q16" s="7">
+      <c r="Q16" s="4">
         <v>2071792</v>
       </c>
-      <c r="R16" s="7">
+      <c r="R16" s="4">
         <v>1133798</v>
       </c>
-      <c r="S16" s="7">
+      <c r="S16" s="4">
         <v>1090250</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="5">
+      <c r="A17" s="9">
         <v>2015</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1518,171 +1519,175 @@
       <c r="C17" s="1">
         <v>82175684</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="4">
         <v>2858714</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="4">
         <v>1787408</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="4">
         <v>7926599</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="4">
         <v>671489</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="4">
         <v>17865516</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="4">
         <v>6176172</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J17" s="4">
         <v>4052803</v>
       </c>
-      <c r="K17" s="7">
+      <c r="K17" s="4">
         <v>10879618</v>
       </c>
-      <c r="L17" s="7">
+      <c r="L17" s="4">
         <v>12843514</v>
       </c>
-      <c r="M17" s="7">
+      <c r="M17" s="4">
         <v>995597</v>
       </c>
-      <c r="N17" s="7">
+      <c r="N17" s="4">
         <v>3520031</v>
       </c>
-      <c r="O17" s="7">
+      <c r="O17" s="4">
         <v>2484826</v>
       </c>
-      <c r="P17" s="7">
+      <c r="P17" s="4">
         <v>1612362</v>
       </c>
-      <c r="Q17" s="7">
+      <c r="Q17" s="4">
         <v>4084851</v>
       </c>
-      <c r="R17" s="7">
+      <c r="R17" s="4">
         <v>2245470</v>
       </c>
-      <c r="S17" s="7">
+      <c r="S17" s="4">
         <v>2170714</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="4"/>
+      <c r="A18" s="9">
+        <v>2015</v>
+      </c>
       <c r="B18" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C18" s="1">
         <v>40514123</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="4">
         <v>1399458</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="4">
         <v>873062</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="4">
         <v>3915398</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="4">
         <v>330895</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H18" s="4">
         <v>8768019</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I18" s="4">
         <v>3047730</v>
       </c>
-      <c r="J18" s="7">
+      <c r="J18" s="4">
         <v>1999333</v>
       </c>
-      <c r="K18" s="7">
+      <c r="K18" s="4">
         <v>5393388</v>
       </c>
-      <c r="L18" s="7">
+      <c r="L18" s="4">
         <v>6352172</v>
       </c>
-      <c r="M18" s="7">
+      <c r="M18" s="4">
         <v>488631</v>
       </c>
-      <c r="N18" s="7">
+      <c r="N18" s="4">
         <v>1726533</v>
       </c>
-      <c r="O18" s="7">
+      <c r="O18" s="4">
         <v>1228283</v>
       </c>
-      <c r="P18" s="7">
+      <c r="P18" s="4">
         <v>797832</v>
       </c>
-      <c r="Q18" s="7">
+      <c r="Q18" s="4">
         <v>2011561</v>
       </c>
-      <c r="R18" s="7">
+      <c r="R18" s="4">
         <v>1106689</v>
       </c>
-      <c r="S18" s="7">
+      <c r="S18" s="4">
         <v>1075139</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="4"/>
+      <c r="A19" s="9">
+        <v>2015</v>
+      </c>
       <c r="B19" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="1">
         <v>41661561</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="4">
         <v>1459256</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="4">
         <v>914346</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="4">
         <v>4011201</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="4">
         <v>340594</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H19" s="4">
         <v>9097497</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I19" s="4">
         <v>3128442</v>
       </c>
-      <c r="J19" s="7">
+      <c r="J19" s="4">
         <v>2053470</v>
       </c>
-      <c r="K19" s="7">
+      <c r="K19" s="4">
         <v>5486230</v>
       </c>
-      <c r="L19" s="7">
+      <c r="L19" s="4">
         <v>6491342</v>
       </c>
-      <c r="M19" s="7">
+      <c r="M19" s="4">
         <v>506966</v>
       </c>
-      <c r="N19" s="7">
+      <c r="N19" s="4">
         <v>1793498</v>
       </c>
-      <c r="O19" s="7">
+      <c r="O19" s="4">
         <v>1256543</v>
       </c>
-      <c r="P19" s="7">
+      <c r="P19" s="4">
         <v>814530</v>
       </c>
-      <c r="Q19" s="7">
+      <c r="Q19" s="4">
         <v>2073290</v>
       </c>
-      <c r="R19" s="7">
+      <c r="R19" s="4">
         <v>1138781</v>
       </c>
-      <c r="S19" s="7">
+      <c r="S19" s="4">
         <v>1095575</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="5">
+      <c r="A20" s="9">
         <v>2014</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1691,171 +1696,175 @@
       <c r="C20" s="1">
         <v>81197537</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="4">
         <v>2830864</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="4">
         <v>1762791</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="4">
         <v>7826739</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="4">
         <v>661888</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H20" s="4">
         <v>17638098</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I20" s="4">
         <v>6093888</v>
       </c>
-      <c r="J20" s="7">
+      <c r="J20" s="4">
         <v>4011582</v>
       </c>
-      <c r="K20" s="7">
+      <c r="K20" s="4">
         <v>10716644</v>
       </c>
-      <c r="L20" s="7">
+      <c r="L20" s="4">
         <v>12691568</v>
       </c>
-      <c r="M20" s="7">
+      <c r="M20" s="4">
         <v>989035</v>
       </c>
-      <c r="N20" s="7">
+      <c r="N20" s="4">
         <v>3469849</v>
       </c>
-      <c r="O20" s="7">
+      <c r="O20" s="4">
         <v>2457872</v>
       </c>
-      <c r="P20" s="7">
+      <c r="P20" s="4">
         <v>1599138</v>
       </c>
-      <c r="Q20" s="7">
+      <c r="Q20" s="4">
         <v>4055274</v>
       </c>
-      <c r="R20" s="7">
+      <c r="R20" s="4">
         <v>2235548</v>
       </c>
-      <c r="S20" s="7">
+      <c r="S20" s="4">
         <v>2156759</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="4"/>
+      <c r="A21" s="9">
+        <v>2014</v>
+      </c>
       <c r="B21" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C21" s="1">
         <v>39835457</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="4">
         <v>1381451</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="4">
         <v>857446</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="4">
         <v>3846089</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="4">
         <v>324423</v>
       </c>
-      <c r="H21" s="7">
+      <c r="H21" s="4">
         <v>8606003</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I21" s="4">
         <v>2991752</v>
       </c>
-      <c r="J21" s="7">
+      <c r="J21" s="4">
         <v>1970535</v>
       </c>
-      <c r="K21" s="7">
+      <c r="K21" s="4">
         <v>5284223</v>
       </c>
-      <c r="L21" s="7">
+      <c r="L21" s="4">
         <v>6249965</v>
       </c>
-      <c r="M21" s="7">
+      <c r="M21" s="4">
         <v>482599</v>
       </c>
-      <c r="N21" s="7">
+      <c r="N21" s="4">
         <v>1696218</v>
       </c>
-      <c r="O21" s="7">
+      <c r="O21" s="4">
         <v>1210474</v>
       </c>
-      <c r="P21" s="7">
+      <c r="P21" s="4">
         <v>787945</v>
       </c>
-      <c r="Q21" s="7">
+      <c r="Q21" s="4">
         <v>1987607</v>
       </c>
-      <c r="R21" s="7">
+      <c r="R21" s="4">
         <v>1095797</v>
       </c>
-      <c r="S21" s="7">
+      <c r="S21" s="4">
         <v>1062930</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="4"/>
+      <c r="A22" s="9">
+        <v>2014</v>
+      </c>
       <c r="B22" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C22" s="1">
         <v>41362080</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="4">
         <v>1449413</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="4">
         <v>905345</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="4">
         <v>3980650</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="4">
         <v>337465</v>
       </c>
-      <c r="H22" s="7">
+      <c r="H22" s="4">
         <v>9032095</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I22" s="4">
         <v>3102136</v>
       </c>
-      <c r="J22" s="7">
+      <c r="J22" s="4">
         <v>2041047</v>
       </c>
-      <c r="K22" s="7">
+      <c r="K22" s="4">
         <v>5432421</v>
       </c>
-      <c r="L22" s="7">
+      <c r="L22" s="4">
         <v>6441603</v>
       </c>
-      <c r="M22" s="7">
+      <c r="M22" s="4">
         <v>506436</v>
       </c>
-      <c r="N22" s="7">
+      <c r="N22" s="4">
         <v>1773631</v>
       </c>
-      <c r="O22" s="7">
+      <c r="O22" s="4">
         <v>1247398</v>
       </c>
-      <c r="P22" s="7">
+      <c r="P22" s="4">
         <v>811193</v>
       </c>
-      <c r="Q22" s="7">
+      <c r="Q22" s="4">
         <v>2067667</v>
       </c>
-      <c r="R22" s="7">
+      <c r="R22" s="4">
         <v>1139751</v>
       </c>
-      <c r="S22" s="7">
+      <c r="S22" s="4">
         <v>1093829</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="5">
+      <c r="A23" s="9">
         <v>2013</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1864,171 +1873,175 @@
       <c r="C23" s="1">
         <v>80767463</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="4">
         <v>2815955</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="4">
         <v>1746342</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="4">
         <v>7790559</v>
       </c>
-      <c r="G23" s="7">
+      <c r="G23" s="4">
         <v>657391</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23" s="4">
         <v>17571856</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I23" s="4">
         <v>6045425</v>
       </c>
-      <c r="J23" s="7">
+      <c r="J23" s="4">
         <v>3994366</v>
       </c>
-      <c r="K23" s="7">
+      <c r="K23" s="4">
         <v>10631278</v>
       </c>
-      <c r="L23" s="7">
+      <c r="L23" s="4">
         <v>12604244</v>
       </c>
-      <c r="M23" s="7">
+      <c r="M23" s="4">
         <v>990718</v>
       </c>
-      <c r="N23" s="7">
+      <c r="N23" s="4">
         <v>3421829</v>
       </c>
-      <c r="O23" s="7">
+      <c r="O23" s="4">
         <v>2449193</v>
       </c>
-      <c r="P23" s="7">
+      <c r="P23" s="4">
         <v>1596505</v>
       </c>
-      <c r="Q23" s="7">
+      <c r="Q23" s="4">
         <v>4046385</v>
       </c>
-      <c r="R23" s="7">
+      <c r="R23" s="4">
         <v>2244577</v>
       </c>
-      <c r="S23" s="7">
+      <c r="S23" s="4">
         <v>2160840</v>
       </c>
     </row>
     <row r="24" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="4"/>
+      <c r="A24" s="9">
+        <v>2013</v>
+      </c>
       <c r="B24" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C24" s="1">
         <v>39556923</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="4">
         <v>1372031</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="4">
         <v>847946</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F24" s="4">
         <v>3821877</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G24" s="4">
         <v>321188</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24" s="4">
         <v>8558968</v>
       </c>
-      <c r="I24" s="7">
+      <c r="I24" s="4">
         <v>2962599</v>
       </c>
-      <c r="J24" s="7">
+      <c r="J24" s="4">
         <v>1958977</v>
       </c>
-      <c r="K24" s="7">
+      <c r="K24" s="4">
         <v>5230706</v>
       </c>
-      <c r="L24" s="7">
+      <c r="L24" s="4">
         <v>6197151</v>
       </c>
-      <c r="M24" s="7">
+      <c r="M24" s="4">
         <v>482434</v>
       </c>
-      <c r="N24" s="7">
+      <c r="N24" s="4">
         <v>1669791</v>
       </c>
-      <c r="O24" s="7">
+      <c r="O24" s="4">
         <v>1205440</v>
       </c>
-      <c r="P24" s="7">
+      <c r="P24" s="4">
         <v>786331</v>
       </c>
-      <c r="Q24" s="7">
+      <c r="Q24" s="4">
         <v>1979164</v>
       </c>
-      <c r="R24" s="7">
+      <c r="R24" s="4">
         <v>1098633</v>
       </c>
-      <c r="S24" s="7">
+      <c r="S24" s="4">
         <v>1063687</v>
       </c>
     </row>
     <row r="25" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="4"/>
+      <c r="A25" s="9">
+        <v>2013</v>
+      </c>
       <c r="B25" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C25" s="1">
         <v>41210540</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="4">
         <v>1443924</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="4">
         <v>898396</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="4">
         <v>3968682</v>
       </c>
-      <c r="G25" s="7">
+      <c r="G25" s="4">
         <v>336203</v>
       </c>
-      <c r="H25" s="7">
+      <c r="H25" s="4">
         <v>9012888</v>
       </c>
-      <c r="I25" s="7">
+      <c r="I25" s="4">
         <v>3082826</v>
       </c>
-      <c r="J25" s="7">
+      <c r="J25" s="4">
         <v>2035389</v>
       </c>
-      <c r="K25" s="7">
+      <c r="K25" s="4">
         <v>5400572</v>
       </c>
-      <c r="L25" s="7">
+      <c r="L25" s="4">
         <v>6407093</v>
       </c>
-      <c r="M25" s="7">
+      <c r="M25" s="4">
         <v>508284</v>
       </c>
-      <c r="N25" s="7">
+      <c r="N25" s="4">
         <v>1752038</v>
       </c>
-      <c r="O25" s="7">
+      <c r="O25" s="4">
         <v>1243753</v>
       </c>
-      <c r="P25" s="7">
+      <c r="P25" s="4">
         <v>810174</v>
       </c>
-      <c r="Q25" s="7">
+      <c r="Q25" s="4">
         <v>2067221</v>
       </c>
-      <c r="R25" s="7">
+      <c r="R25" s="4">
         <v>1145944</v>
       </c>
-      <c r="S25" s="7">
+      <c r="S25" s="4">
         <v>1097153</v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="5">
+      <c r="A26" s="9">
         <v>2012</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -2037,171 +2050,175 @@
       <c r="C26" s="1">
         <v>80523746</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="4">
         <v>2806531</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="4">
         <v>1734272</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="4">
         <v>7778995</v>
       </c>
-      <c r="G26" s="7">
+      <c r="G26" s="4">
         <v>654774</v>
       </c>
-      <c r="H26" s="7">
+      <c r="H26" s="4">
         <v>17554329</v>
       </c>
-      <c r="I26" s="7">
+      <c r="I26" s="4">
         <v>6016481</v>
       </c>
-      <c r="J26" s="7">
+      <c r="J26" s="4">
         <v>3990278</v>
       </c>
-      <c r="K26" s="7">
+      <c r="K26" s="4">
         <v>10569111</v>
       </c>
-      <c r="L26" s="7">
+      <c r="L26" s="4">
         <v>12519571</v>
       </c>
-      <c r="M26" s="7">
+      <c r="M26" s="4">
         <v>994287</v>
       </c>
-      <c r="N26" s="7">
+      <c r="N26" s="4">
         <v>3375222</v>
       </c>
-      <c r="O26" s="7">
+      <c r="O26" s="4">
         <v>2449511</v>
       </c>
-      <c r="P26" s="7">
+      <c r="P26" s="4">
         <v>1600327</v>
       </c>
-      <c r="Q26" s="7">
+      <c r="Q26" s="4">
         <v>4050204</v>
       </c>
-      <c r="R26" s="7">
+      <c r="R26" s="4">
         <v>2259393</v>
       </c>
-      <c r="S26" s="7">
+      <c r="S26" s="4">
         <v>2170460</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="4"/>
+      <c r="A27" s="9">
+        <v>2012</v>
+      </c>
       <c r="B27" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C27" s="1">
         <v>39380976</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="4">
         <v>1365954</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="4">
         <v>841246</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="4">
         <v>3811002</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="4">
         <v>319065</v>
       </c>
-      <c r="H27" s="7">
+      <c r="H27" s="4">
         <v>8540059</v>
       </c>
-      <c r="I27" s="7">
+      <c r="I27" s="4">
         <v>2943034</v>
       </c>
-      <c r="J27" s="7">
+      <c r="J27" s="4">
         <v>1954161</v>
       </c>
-      <c r="K27" s="7">
+      <c r="K27" s="4">
         <v>5189475</v>
       </c>
-      <c r="L27" s="7">
+      <c r="L27" s="4">
         <v>6143980</v>
       </c>
-      <c r="M27" s="7">
+      <c r="M27" s="4">
         <v>483558</v>
       </c>
-      <c r="N27" s="7">
+      <c r="N27" s="4">
         <v>1644451</v>
       </c>
-      <c r="O27" s="7">
+      <c r="O27" s="4">
         <v>1205360</v>
       </c>
-      <c r="P27" s="7">
+      <c r="P27" s="4">
         <v>788104</v>
       </c>
-      <c r="Q27" s="7">
+      <c r="Q27" s="4">
         <v>1978504</v>
       </c>
-      <c r="R27" s="7">
+      <c r="R27" s="4">
         <v>1104896</v>
       </c>
-      <c r="S27" s="7">
+      <c r="S27" s="4">
         <v>1068127</v>
       </c>
     </row>
     <row r="28" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="4"/>
+      <c r="A28" s="9">
+        <v>2012</v>
+      </c>
       <c r="B28" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C28" s="1">
         <v>41142770</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="4">
         <v>1440577</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="4">
         <v>893026</v>
       </c>
-      <c r="F28" s="7">
+      <c r="F28" s="4">
         <v>3967993</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G28" s="4">
         <v>335709</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H28" s="4">
         <v>9014270</v>
       </c>
-      <c r="I28" s="7">
+      <c r="I28" s="4">
         <v>3073447</v>
       </c>
-      <c r="J28" s="7">
+      <c r="J28" s="4">
         <v>2036117</v>
       </c>
-      <c r="K28" s="7">
+      <c r="K28" s="4">
         <v>5379636</v>
       </c>
-      <c r="L28" s="7">
+      <c r="L28" s="4">
         <v>6375591</v>
       </c>
-      <c r="M28" s="7">
+      <c r="M28" s="4">
         <v>510729</v>
       </c>
-      <c r="N28" s="7">
+      <c r="N28" s="4">
         <v>1730771</v>
       </c>
-      <c r="O28" s="7">
+      <c r="O28" s="4">
         <v>1244151</v>
       </c>
-      <c r="P28" s="7">
+      <c r="P28" s="4">
         <v>812223</v>
       </c>
-      <c r="Q28" s="7">
+      <c r="Q28" s="4">
         <v>2071700</v>
       </c>
-      <c r="R28" s="7">
+      <c r="R28" s="4">
         <v>1154497</v>
       </c>
-      <c r="S28" s="7">
+      <c r="S28" s="4">
         <v>1102333</v>
       </c>
     </row>
     <row r="29" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="5">
+      <c r="A29" s="9">
         <v>2011</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -2210,171 +2227,175 @@
       <c r="C29" s="1">
         <v>80327900</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="4">
         <v>2802266</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="4">
         <v>1718187</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="4">
         <v>7774253</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G29" s="4">
         <v>652182</v>
       </c>
-      <c r="H29" s="7">
+      <c r="H29" s="4">
         <v>17544938</v>
       </c>
-      <c r="I29" s="7">
+      <c r="I29" s="4">
         <v>5993771</v>
       </c>
-      <c r="J29" s="7">
+      <c r="J29" s="4">
         <v>3990033</v>
       </c>
-      <c r="K29" s="7">
+      <c r="K29" s="4">
         <v>10512441</v>
       </c>
-      <c r="L29" s="7">
+      <c r="L29" s="4">
         <v>12443372</v>
       </c>
-      <c r="M29" s="7">
+      <c r="M29" s="4">
         <v>997855</v>
       </c>
-      <c r="N29" s="7">
+      <c r="N29" s="4">
         <v>3326002</v>
       </c>
-      <c r="O29" s="7">
+      <c r="O29" s="4">
         <v>2453180</v>
       </c>
-      <c r="P29" s="7">
+      <c r="P29" s="4">
         <v>1606899</v>
       </c>
-      <c r="Q29" s="7">
+      <c r="Q29" s="4">
         <v>4054182</v>
       </c>
-      <c r="R29" s="7">
+      <c r="R29" s="4">
         <v>2276736</v>
       </c>
-      <c r="S29" s="7">
+      <c r="S29" s="4">
         <v>2181603</v>
       </c>
     </row>
     <row r="30" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="4"/>
+      <c r="A30" s="9">
+        <v>2011</v>
+      </c>
       <c r="B30" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C30" s="1">
         <v>39229947</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="4">
         <v>1362391</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="4">
         <v>832064</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="4">
         <v>3803884</v>
       </c>
-      <c r="G30" s="7">
+      <c r="G30" s="4">
         <v>317060</v>
       </c>
-      <c r="H30" s="7">
+      <c r="H30" s="4">
         <v>8525378</v>
       </c>
-      <c r="I30" s="7">
+      <c r="I30" s="4">
         <v>2927628</v>
       </c>
-      <c r="J30" s="7">
+      <c r="J30" s="4">
         <v>1951624</v>
       </c>
-      <c r="K30" s="7">
+      <c r="K30" s="4">
         <v>5151354</v>
       </c>
-      <c r="L30" s="7">
+      <c r="L30" s="4">
         <v>6093411</v>
       </c>
-      <c r="M30" s="7">
+      <c r="M30" s="4">
         <v>484604</v>
       </c>
-      <c r="N30" s="7">
+      <c r="N30" s="4">
         <v>1617768</v>
       </c>
-      <c r="O30" s="7">
+      <c r="O30" s="4">
         <v>1207189</v>
       </c>
-      <c r="P30" s="7">
+      <c r="P30" s="4">
         <v>791635</v>
       </c>
-      <c r="Q30" s="7">
+      <c r="Q30" s="4">
         <v>1978178</v>
       </c>
-      <c r="R30" s="7">
+      <c r="R30" s="4">
         <v>1112710</v>
       </c>
-      <c r="S30" s="7">
+      <c r="S30" s="4">
         <v>1073069</v>
       </c>
     </row>
     <row r="31" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="4"/>
+      <c r="A31" s="9">
+        <v>2011</v>
+      </c>
       <c r="B31" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C31" s="1">
         <v>41097953</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D31" s="4">
         <v>1439875</v>
       </c>
-      <c r="E31" s="7">
+      <c r="E31" s="4">
         <v>886123</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="4">
         <v>3970369</v>
       </c>
-      <c r="G31" s="7">
+      <c r="G31" s="4">
         <v>335122</v>
       </c>
-      <c r="H31" s="7">
+      <c r="H31" s="4">
         <v>9019560</v>
       </c>
-      <c r="I31" s="7">
+      <c r="I31" s="4">
         <v>3066143</v>
       </c>
-      <c r="J31" s="7">
+      <c r="J31" s="4">
         <v>2038409</v>
       </c>
-      <c r="K31" s="7">
+      <c r="K31" s="4">
         <v>5361087</v>
       </c>
-      <c r="L31" s="7">
+      <c r="L31" s="4">
         <v>6349961</v>
       </c>
-      <c r="M31" s="7">
+      <c r="M31" s="4">
         <v>513251</v>
       </c>
-      <c r="N31" s="7">
+      <c r="N31" s="4">
         <v>1708234</v>
       </c>
-      <c r="O31" s="7">
+      <c r="O31" s="4">
         <v>1245991</v>
       </c>
-      <c r="P31" s="7">
+      <c r="P31" s="4">
         <v>815264</v>
       </c>
-      <c r="Q31" s="7">
+      <c r="Q31" s="4">
         <v>2076004</v>
       </c>
-      <c r="R31" s="7">
+      <c r="R31" s="4">
         <v>1164026</v>
       </c>
-      <c r="S31" s="7">
+      <c r="S31" s="4">
         <v>1108534</v>
       </c>
     </row>
     <row r="32" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="5">
+      <c r="A32" s="9">
         <v>2010</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -2383,183 +2404,174 @@
       <c r="C32" s="1">
         <v>81751602</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="4">
         <v>2834259</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="4">
         <v>1786448</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="4">
         <v>7918293</v>
       </c>
-      <c r="G32" s="7">
+      <c r="G32" s="4">
         <v>660706</v>
       </c>
-      <c r="H32" s="7">
+      <c r="H32" s="4">
         <v>17845154</v>
       </c>
-      <c r="I32" s="7">
+      <c r="I32" s="4">
         <v>6067021</v>
       </c>
-      <c r="J32" s="7">
+      <c r="J32" s="4">
         <v>4003745</v>
       </c>
-      <c r="K32" s="7">
+      <c r="K32" s="4">
         <v>10753880</v>
       </c>
-      <c r="L32" s="7">
+      <c r="L32" s="4">
         <v>12538696</v>
       </c>
-      <c r="M32" s="7">
+      <c r="M32" s="4">
         <v>1017567</v>
       </c>
-      <c r="N32" s="7">
+      <c r="N32" s="4">
         <v>3460725</v>
       </c>
-      <c r="O32" s="7">
+      <c r="O32" s="4">
         <v>2503273</v>
       </c>
-      <c r="P32" s="7">
+      <c r="P32" s="4">
         <v>1642327</v>
       </c>
-      <c r="Q32" s="7">
+      <c r="Q32" s="4">
         <v>4149477</v>
       </c>
-      <c r="R32" s="7">
+      <c r="R32" s="4">
         <v>2335006</v>
       </c>
-      <c r="S32" s="7">
+      <c r="S32" s="4">
         <v>2235025</v>
       </c>
     </row>
     <row r="33" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="4"/>
+      <c r="A33" s="9">
+        <v>2010</v>
+      </c>
       <c r="B33" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C33" s="1">
         <v>40112425</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="4">
         <v>1388912</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33" s="4">
         <v>873712</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F33" s="4">
         <v>3893761</v>
       </c>
-      <c r="G33" s="7">
+      <c r="G33" s="4">
         <v>321940</v>
       </c>
-      <c r="H33" s="7">
+      <c r="H33" s="4">
         <v>8711858</v>
       </c>
-      <c r="I33" s="7">
+      <c r="I33" s="4">
         <v>2976527</v>
       </c>
-      <c r="J33" s="7">
+      <c r="J33" s="4">
         <v>1967106</v>
       </c>
-      <c r="K33" s="7">
+      <c r="K33" s="4">
         <v>5296249</v>
       </c>
-      <c r="L33" s="7">
+      <c r="L33" s="4">
         <v>6158439</v>
       </c>
-      <c r="M33" s="7">
+      <c r="M33" s="4">
         <v>495206</v>
       </c>
-      <c r="N33" s="7">
+      <c r="N33" s="4">
         <v>1695438</v>
       </c>
-      <c r="O33" s="7">
+      <c r="O33" s="4">
         <v>1240553</v>
       </c>
-      <c r="P33" s="7">
+      <c r="P33" s="4">
         <v>813283</v>
       </c>
-      <c r="Q33" s="7">
+      <c r="Q33" s="4">
         <v>2031630</v>
       </c>
-      <c r="R33" s="7">
+      <c r="R33" s="4">
         <v>1144118</v>
       </c>
-      <c r="S33" s="7">
+      <c r="S33" s="4">
         <v>1103693</v>
       </c>
     </row>
     <row r="34" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="6"/>
+      <c r="A34" s="9">
+        <v>2010</v>
+      </c>
       <c r="B34" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C34" s="1">
         <v>41639177</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="4">
         <v>1445347</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="4">
         <v>912736</v>
       </c>
-      <c r="F34" s="7">
+      <c r="F34" s="4">
         <v>4024532</v>
       </c>
-      <c r="G34" s="7">
+      <c r="G34" s="4">
         <v>338766</v>
       </c>
-      <c r="H34" s="7">
+      <c r="H34" s="4">
         <v>9133296</v>
       </c>
-      <c r="I34" s="7">
+      <c r="I34" s="4">
         <v>3090494</v>
       </c>
-      <c r="J34" s="7">
+      <c r="J34" s="4">
         <v>2036639</v>
       </c>
-      <c r="K34" s="7">
+      <c r="K34" s="4">
         <v>5457631</v>
       </c>
-      <c r="L34" s="7">
+      <c r="L34" s="4">
         <v>6380257</v>
       </c>
-      <c r="M34" s="7">
+      <c r="M34" s="4">
         <v>522361</v>
       </c>
-      <c r="N34" s="7">
+      <c r="N34" s="4">
         <v>1765287</v>
       </c>
-      <c r="O34" s="7">
+      <c r="O34" s="4">
         <v>1262720</v>
       </c>
-      <c r="P34" s="7">
+      <c r="P34" s="4">
         <v>829044</v>
       </c>
-      <c r="Q34" s="7">
+      <c r="Q34" s="4">
         <v>2117847</v>
       </c>
-      <c r="R34" s="7">
+      <c r="R34" s="4">
         <v>1190888</v>
       </c>
-      <c r="S34" s="7">
+      <c r="S34" s="4">
         <v>1131332</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A17:A19"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>